<commit_message>
madke changes to add input
</commit_message>
<xml_diff>
--- a/inventory_project/inventory_app/static/inventory_app/Inventory.xlsx
+++ b/inventory_project/inventory_app/static/inventory_app/Inventory.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1988" uniqueCount="1058">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1997" uniqueCount="1060">
   <si>
     <t>Part_Name</t>
   </si>
@@ -3187,7 +3187,13 @@
     <t>TRAILBLAZER</t>
   </si>
   <si>
-    <t>29-03-2024 22:49</t>
+    <t>31-03-2024 01:34</t>
+  </si>
+  <si>
+    <t>31-03-2024 01:35</t>
+  </si>
+  <si>
+    <t>31-03-2024 11:16</t>
   </si>
 </sst>
 </file>
@@ -3549,7 +3555,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F661"/>
+  <dimension ref="A1:F663"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -16775,6 +16781,46 @@
         <v>1057</v>
       </c>
     </row>
+    <row r="662" spans="1:6">
+      <c r="A662" t="s">
+        <v>394</v>
+      </c>
+      <c r="B662" t="s">
+        <v>394</v>
+      </c>
+      <c r="C662" t="s">
+        <v>394</v>
+      </c>
+      <c r="D662" t="s">
+        <v>394</v>
+      </c>
+      <c r="E662">
+        <v>66</v>
+      </c>
+      <c r="F662" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="663" spans="1:6">
+      <c r="A663" t="s">
+        <v>394</v>
+      </c>
+      <c r="B663">
+        <v>2200</v>
+      </c>
+      <c r="C663" t="s">
+        <v>394</v>
+      </c>
+      <c r="D663" t="s">
+        <v>394</v>
+      </c>
+      <c r="E663">
+        <v>792</v>
+      </c>
+      <c r="F663" t="s">
+        <v>1059</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>